<commit_message>
Added priority, risk/value and points to the stories derived from the additional requirements
As we were busy with the sprint we just left the priority as TBD as we would work that out when planning for next sprint
</commit_message>
<xml_diff>
--- a/ProductBacklog/Product Backlog.xlsx
+++ b/ProductBacklog/Product Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
   <si>
     <t>Group 9 Product Backlog</t>
   </si>
@@ -97,33 +97,33 @@
     <t>View it on the go or without the use of a computer</t>
   </si>
   <si>
+    <t>Use my current location to see nearby events</t>
+  </si>
+  <si>
+    <t>Participate in nearby events so that I can participate in events close to me</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Intergrate with my social media</t>
+  </si>
+  <si>
+    <t>Check into a location through my social media feed</t>
+  </si>
+  <si>
+    <t>Back-End User</t>
+  </si>
+  <si>
+    <t>Create new items</t>
+  </si>
+  <si>
+    <t>Add new events onto the website</t>
+  </si>
+  <si>
     <t>In Progress</t>
   </si>
   <si>
-    <t>Use my current location to see nearby events</t>
-  </si>
-  <si>
-    <t>Participate in nearby events so that I can participate in events close to me</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Intergrate with my social media</t>
-  </si>
-  <si>
-    <t>Check into a location through my social media feed</t>
-  </si>
-  <si>
-    <t>Back-End User</t>
-  </si>
-  <si>
-    <t>Create new items</t>
-  </si>
-  <si>
-    <t>Add new events onto the website</t>
-  </si>
-  <si>
     <t>Edit current events</t>
   </si>
   <si>
@@ -151,26 +151,32 @@
     <t>Bring more awareness to an upcoming event</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Create tours of events</t>
   </si>
   <si>
     <t>Other users can easily see where all the goals will be taking place</t>
   </si>
   <si>
+    <t>High/Low</t>
+  </si>
+  <si>
     <t>Check into venues and see a leaderboard of other users check ins</t>
   </si>
   <si>
     <t>Compare my commitment to a goal to other users</t>
+  </si>
+  <si>
+    <t>Access a map of events that are related to a goal that I am interested in</t>
+  </si>
+  <si>
+    <t>See which events are in my area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -182,6 +188,10 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -257,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border/>
     <border>
       <left/>
@@ -265,11 +275,6 @@
       <bottom/>
     </border>
     <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
       <top/>
       <bottom/>
     </border>
@@ -283,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -291,26 +296,58 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="7" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="8" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="9" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="6" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="10" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="10" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="11" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="11" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="12" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -546,399 +583,424 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>1.0</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <v>3.0</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>2.0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>3.0</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>3.0</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <v>2.0</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>4.0</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>5.0</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>5.0</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>1.0</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>28</v>
+      <c r="J8" s="14" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>6.0</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>14</v>
+      <c r="J9" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>7.0</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="11">
         <v>1.0</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>8.0</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="J11" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>9.0</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="11">
         <v>3.0</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>10.0</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="11">
         <v>2.0</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>11.0</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="11">
         <v>13.0</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>13.0</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="15" t="s">
+      <c r="G15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="J15" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>14.0</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="D16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="15" t="s">
+      <c r="I16" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>15.0</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="15" t="s">
+      <c r="G17" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="C18" s="20">
+        <v>24.0</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="25">
+        <v>13.0</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updated to reflect sprint progress
</commit_message>
<xml_diff>
--- a/ProductBacklog/Product Backlog.xlsx
+++ b/ProductBacklog/Product Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Submit Later\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Day 2 Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,14 +274,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -318,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -337,7 +343,6 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -347,12 +352,14 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,8 +585,8 @@
   </sheetPr>
   <dimension ref="C1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -593,16 +600,16 @@
   <sheetData>
     <row r="1" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
@@ -730,8 +737,8 @@
       <c r="I7" s="9">
         <v>5</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>25</v>
+      <c r="J7" s="26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -808,8 +815,8 @@
       <c r="I10" s="9">
         <v>1</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>25</v>
+      <c r="J10" s="26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -834,7 +841,7 @@
       <c r="I11" s="9">
         <v>5</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="23" t="s">
         <v>14</v>
       </c>
     </row>
@@ -860,8 +867,8 @@
       <c r="I12" s="9">
         <v>3</v>
       </c>
-      <c r="J12" s="14" t="s">
-        <v>36</v>
+      <c r="J12" s="23" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -912,7 +919,7 @@
       <c r="I14" s="9">
         <v>13</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="23" t="s">
         <v>14</v>
       </c>
     </row>
@@ -929,17 +936,17 @@
       <c r="F15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="16">
         <v>1</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>25</v>
+      <c r="J15" s="27" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -955,17 +962,17 @@
       <c r="F16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="16">
         <v>3</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>25</v>
+      <c r="J16" s="26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -981,13 +988,13 @@
       <c r="F17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="16" t="s">
         <v>30</v>
       </c>
       <c r="J17" s="11" t="s">
@@ -995,29 +1002,29 @@
       </c>
     </row>
     <row r="18" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="18">
+      <c r="C18" s="17">
         <v>24</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="22">
         <v>13</v>
       </c>
-      <c r="J18" s="24" t="s">
-        <v>25</v>
+      <c r="J18" s="28" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>